<commit_message>
Add Documentation to Codes and Update the Excel Output
</commit_message>
<xml_diff>
--- a/output/reviewSentiment20.xlsx
+++ b/output/reviewSentiment20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wu_ziang/Desktop/AY1920S1/CZ4045 Natural Language Processing/Assignment/NLP Workspace/sentiment_analysis/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wu_ziang/Desktop/AY1920S1/CZ4045 Natural Language Processing/Assignment/Assignment/NTU-20191011/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB79D32D-A2C9-134B-9978-46A2C23CEA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9541029-6B31-B641-95FB-872AAD67B9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="0" windowWidth="17960" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="0" windowWidth="26220" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,48 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="175">
   <si>
-    <t>review_id</t>
-  </si>
-  <si>
-    <t>business_id</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>stars</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>sentences</t>
-  </si>
-  <si>
-    <t>word_count</t>
-  </si>
-  <si>
-    <t>score_vader</t>
-  </si>
-  <si>
-    <t>weighted_vader</t>
-  </si>
-  <si>
-    <t>score_flair</t>
-  </si>
-  <si>
-    <t>weighted_flair</t>
-  </si>
-  <si>
-    <t>negex_vader</t>
-  </si>
-  <si>
-    <t>negex_flair</t>
-  </si>
-  <si>
     <t>fdiNeiN_hoCxCMy2wTRW9g</t>
   </si>
   <si>
@@ -580,6 +538,48 @@
   </si>
   <si>
     <t>[0.9987, -0.6351, 0.8961, 0.9928, -0.5044, 0.5829, 0.6741, 0.7897]</t>
+  </si>
+  <si>
+    <t>Review ID</t>
+  </si>
+  <si>
+    <t>Business ID</t>
+  </si>
+  <si>
+    <t>USER ID</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Sentences</t>
+  </si>
+  <si>
+    <t>Word Count</t>
+  </si>
+  <si>
+    <t>Score Vader</t>
+  </si>
+  <si>
+    <t>Weighted Vader</t>
+  </si>
+  <si>
+    <t>Score Flair</t>
+  </si>
+  <si>
+    <t>Weighted Flair</t>
+  </si>
+  <si>
+    <t>Sentiment Vader</t>
+  </si>
+  <si>
+    <t>Sentiment Flair</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,13 +602,30 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -638,12 +655,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,997 +1026,1012 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="80.83203125" style="7" customWidth="1"/>
+    <col min="9" max="10" width="30.83203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="12" width="30.83203125" style="11" customWidth="1"/>
+    <col min="13" max="15" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="G2" s="2">
         <v>41294.559710648151</v>
       </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
+      <c r="H2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="K2">
         <v>0.20710697674418599</v>
       </c>
-      <c r="L2" t="s">
-        <v>21</v>
+      <c r="L2" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="M2">
         <v>0.66277940199335517</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>26</v>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="2">
         <v>42497.056273148148</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
+      <c r="H3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="K3">
         <v>0.3025353413654619</v>
       </c>
-      <c r="L3" t="s">
-        <v>30</v>
+      <c r="L3" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="M3">
         <v>0.29440040160642572</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="2">
         <v>42881.057858796303</v>
       </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" t="s">
-        <v>37</v>
+      <c r="H4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="K4">
         <v>0.61790624999999999</v>
       </c>
-      <c r="L4" t="s">
-        <v>38</v>
+      <c r="L4" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="M4">
         <v>0.682925</v>
       </c>
       <c r="N4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>42</v>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G5" s="2">
         <v>41817.897581018522</v>
       </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
+      <c r="H5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="K5">
         <v>-0.1486446153846154</v>
       </c>
-      <c r="L5" t="s">
-        <v>46</v>
+      <c r="L5" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="M5">
         <v>-0.48456584615384612</v>
       </c>
       <c r="N5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6">
+      <c r="B6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="15">
         <v>42343.1090625</v>
       </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6">
+      <c r="H6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="13">
         <v>-6.0673529411764703E-2</v>
       </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6">
+      <c r="L6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="13">
         <v>0.99696176470588227</v>
       </c>
-      <c r="N6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" t="s">
-        <v>22</v>
+      <c r="N6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>59</v>
+      <c r="F7" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="G7" s="2">
         <v>41907.344259259262</v>
       </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" t="s">
-        <v>62</v>
+      <c r="H7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="K7">
         <v>0.10835208333333329</v>
       </c>
-      <c r="L7" t="s">
-        <v>63</v>
+      <c r="L7" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="M7">
         <v>0.6299083333333334</v>
       </c>
       <c r="N7" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O7" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
-        <v>66</v>
+      <c r="F8" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="G8" s="2">
         <v>41939.182337962957</v>
       </c>
-      <c r="H8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" t="s">
-        <v>69</v>
+      <c r="H8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="K8">
         <v>0.45928768844221107</v>
       </c>
-      <c r="L8" t="s">
-        <v>70</v>
+      <c r="L8" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="M8">
         <v>8.2624874371859322E-2</v>
       </c>
       <c r="N8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>74</v>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G9" s="2">
         <v>41675.755057870367</v>
       </c>
-      <c r="H9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" t="s">
-        <v>77</v>
+      <c r="H9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="K9">
         <v>0.190525</v>
       </c>
-      <c r="L9" t="s">
-        <v>78</v>
+      <c r="L9" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="M9">
         <v>0.63459583333333325</v>
       </c>
       <c r="N9" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O9" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>82</v>
+      <c r="F10" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="G10" s="2">
         <v>42576.163425925923</v>
       </c>
-      <c r="H10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" t="s">
-        <v>85</v>
+      <c r="H10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="K10">
         <v>0.17218090909090911</v>
       </c>
-      <c r="L10" t="s">
-        <v>86</v>
+      <c r="L10" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="M10">
         <v>1.913545454545458E-2</v>
       </c>
       <c r="N10" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O10" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
-        <v>90</v>
+      <c r="F11" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="G11" s="2">
         <v>43205.48233796296</v>
       </c>
-      <c r="H11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" t="s">
-        <v>93</v>
+      <c r="H11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="K11">
         <v>0.55332631578947367</v>
       </c>
-      <c r="L11" t="s">
-        <v>94</v>
+      <c r="L11" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="M11">
         <v>-0.86201052631578945</v>
       </c>
       <c r="N11" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O11" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12">
+      <c r="B12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="13">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="F12" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="15">
         <v>42201.236493055563</v>
       </c>
-      <c r="H12" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" t="s">
-        <v>100</v>
-      </c>
-      <c r="J12" t="s">
-        <v>101</v>
-      </c>
-      <c r="K12">
+      <c r="H12" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="13">
         <v>9.1747417840375572E-2</v>
       </c>
-      <c r="L12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M12">
+      <c r="L12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="13">
         <v>-0.33956338028169009</v>
       </c>
-      <c r="N12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" t="s">
-        <v>47</v>
+      <c r="N12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E13">
         <v>5</v>
       </c>
-      <c r="F13" t="s">
-        <v>106</v>
+      <c r="F13" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="G13" s="2">
         <v>41247.146192129629</v>
       </c>
-      <c r="H13" t="s">
-        <v>107</v>
-      </c>
-      <c r="I13" t="s">
-        <v>108</v>
-      </c>
-      <c r="J13" t="s">
-        <v>109</v>
+      <c r="H13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="K13">
         <v>0.53232222222222225</v>
       </c>
-      <c r="L13" t="s">
-        <v>110</v>
+      <c r="L13" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="M13">
         <v>0.91832962962962961</v>
       </c>
       <c r="N13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="E14">
         <v>5</v>
       </c>
-      <c r="F14" t="s">
-        <v>114</v>
+      <c r="F14" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="G14" s="2">
         <v>40552.005046296297</v>
       </c>
-      <c r="H14" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" t="s">
-        <v>117</v>
+      <c r="H14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="K14">
         <v>0.31047769230769229</v>
       </c>
-      <c r="L14" t="s">
-        <v>118</v>
+      <c r="L14" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="M14">
         <v>0.39849692307692308</v>
       </c>
       <c r="N14" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O14" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="15" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="19">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="20">
+        <v>5</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="22">
+        <v>40587.740914351853</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="20">
+        <v>0.89112666666666662</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="20">
+        <v>-0.87855047619047621</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="15">
+        <v>41422.859872685192</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J16" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C15" t="s">
+      <c r="K16" s="13">
+        <v>1.584166666666666E-2</v>
+      </c>
+      <c r="L16" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G15" s="2">
-        <v>40587.740914351853</v>
-      </c>
-      <c r="H15" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J15" t="s">
-        <v>125</v>
-      </c>
-      <c r="K15">
-        <v>0.89112666666666662</v>
-      </c>
-      <c r="L15" t="s">
-        <v>126</v>
-      </c>
-      <c r="M15">
-        <v>-0.87855047619047621</v>
-      </c>
-      <c r="N15" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" t="s">
-        <v>47</v>
+      <c r="M16" s="13">
+        <v>-0.47324166666666662</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="2">
-        <v>41422.859872685192</v>
-      </c>
-      <c r="H16" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" t="s">
-        <v>132</v>
-      </c>
-      <c r="J16" t="s">
-        <v>133</v>
-      </c>
-      <c r="K16">
-        <v>1.584166666666666E-2</v>
-      </c>
-      <c r="L16" t="s">
-        <v>134</v>
-      </c>
-      <c r="M16">
-        <v>-0.47324166666666662</v>
-      </c>
-      <c r="N16" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
-        <v>138</v>
+      <c r="F17" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="G17" s="2">
         <v>43316.858969907407</v>
       </c>
-      <c r="H17" t="s">
-        <v>139</v>
-      </c>
-      <c r="I17" t="s">
-        <v>140</v>
-      </c>
-      <c r="J17" t="s">
-        <v>141</v>
+      <c r="H17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="K17">
         <v>0.10403913043478261</v>
       </c>
-      <c r="L17" t="s">
-        <v>142</v>
+      <c r="L17" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="M17">
         <v>0.22668840579710151</v>
       </c>
       <c r="N17" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O17" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>146</v>
+      <c r="F18" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="G18" s="2">
         <v>43174.842118055552</v>
       </c>
-      <c r="H18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18" t="s">
-        <v>148</v>
-      </c>
-      <c r="J18" t="s">
-        <v>149</v>
+      <c r="H18" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="K18">
         <v>0.13210134228187931</v>
       </c>
-      <c r="L18" t="s">
-        <v>150</v>
+      <c r="L18" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="M18">
         <v>-0.17894429530201339</v>
       </c>
       <c r="N18" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O18" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E19">
         <v>2</v>
       </c>
-      <c r="F19" t="s">
-        <v>154</v>
+      <c r="F19" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="G19" s="2">
         <v>41656.016296296293</v>
       </c>
-      <c r="H19" t="s">
-        <v>155</v>
-      </c>
-      <c r="I19" t="s">
-        <v>156</v>
-      </c>
-      <c r="J19" t="s">
-        <v>157</v>
+      <c r="H19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="K19">
         <v>-0.1455217948717949</v>
       </c>
-      <c r="L19" t="s">
-        <v>158</v>
+      <c r="L19" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="M19">
         <v>-0.28940205128205132</v>
       </c>
       <c r="N19" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="O19" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E20">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
-        <v>162</v>
+      <c r="F20" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="G20" s="2">
         <v>43248.855868055558</v>
       </c>
-      <c r="H20" t="s">
-        <v>163</v>
-      </c>
-      <c r="I20" t="s">
-        <v>164</v>
-      </c>
-      <c r="J20" t="s">
-        <v>165</v>
+      <c r="H20" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="K20">
         <v>0.3899617647058824</v>
       </c>
-      <c r="L20" t="s">
-        <v>166</v>
+      <c r="L20" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="M20">
         <v>0.34569705882352941</v>
       </c>
       <c r="N20" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O20" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
-      <c r="F21" t="s">
-        <v>170</v>
+      <c r="F21" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="G21" s="2">
         <v>42007.94903935185</v>
       </c>
-      <c r="H21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I21" t="s">
-        <v>172</v>
-      </c>
-      <c r="J21" t="s">
-        <v>173</v>
+      <c r="H21" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="K21">
         <v>0.28283553719008259</v>
       </c>
-      <c r="L21" t="s">
-        <v>174</v>
+      <c r="L21" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="M21">
         <v>8.6526446280991751E-2</v>
       </c>
       <c r="N21" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O21" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>